<commit_message>
Committing new results for AvailableWorkers (UniformTasks_1000_T07). Committing xlsx files for previous results.
</commit_message>
<xml_diff>
--- a/SCFrameworkImpl/Results/TaskRate/UniformTasks_1000_W10/UniformTasks_1000_W10.xlsx
+++ b/SCFrameworkImpl/Results/TaskRate/UniformTasks_1000_W10/UniformTasks_1000_W10.xlsx
@@ -546,6 +546,1384 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Rnk</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>14.275</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.029999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.434999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.639999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.789999999999992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.545000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63.544999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68.324999999999974</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.41</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72.850000000000009</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>76.17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>76.13000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>78.860000000000014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>79.914999999999992</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80.984999999999985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>82.294999999999987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82.74</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>83.84</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>84.195000000000022</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>85.759999999999977</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>86.544999999999987</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>86.965000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>87.54</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>88.455000000000013</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>89.010000000000019</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>88.740000000000023</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>89.580000000000013</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>89.534999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>89.940000000000012</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>91.635000000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>91.885000000000019</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>92.594999999999985</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>92.749999999999986</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>92.775000000000006</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>92.82</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>92.929999999999993</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>93.609999999999985</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>93.28</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>93.580000000000013</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>92.84</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>93.405000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>93.200000000000017</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>93.484999999999985</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>93.375000000000028</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>93.329999999999984</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>93.414999999999992</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>93.089999999999989</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>NN</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>14.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.844999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.804999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.889999999999986</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.849999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80.924999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.754999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.109999999999985</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.324999999999989</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>89.085000000000008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.995000000000019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90.81</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90.965000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91.295000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>92.775000000000006</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>92.674999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>93.435000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>93.60499999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>93.78</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>94.449999999999974</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>94.029999999999987</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>94.73</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>94.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>94.78</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>95.739999999999981</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>95.499999999999986</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>95.474999999999994</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>95.555000000000007</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95.329999999999984</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95.24499999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.049999999999983</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>95.444999999999965</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95.179999999999978</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95.304999999999993</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>94.760000000000019</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>95.14</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>94.775000000000006</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>94.70999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>94.649999999999991</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94.624999999999972</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>94.26</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BI</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>14.805000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.364999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.655000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.655000000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.984999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.474999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.820000000000022</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80.894999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.094999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>87.064999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88.02000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>91.125</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91.41</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>92.61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>93.109999999999985</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>93.34999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>93.73</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95.07</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>94.740000000000009</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>95.679999999999993</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>95.404999999999987</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>95.640000000000015</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>96.034999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96.075000000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>96.135000000000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>96.169999999999987</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>96.45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>96.915000000000006</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>96.36</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>96.369999999999976</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>96.205000000000013</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95.935000000000016</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95.720000000000013</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.605000000000004</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>95.820000000000022</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95.47999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95.59</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>95.02500000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>95.335000000000008</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>95.055000000000007</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>94.955000000000013</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>94.85499999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.825000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94.685000000000002</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>94.42</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>BD</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>14.860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.335000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.524999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.340000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.080000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69.935000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.754999999999967</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.155000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80.569999999999993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.324999999999989</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.989999999999981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.815000000000012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.260000000000019</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>89.01</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.66</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>91.00500000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>91.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91.835000000000008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>93.009999999999991</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>92.95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>93.85</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>94.37</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>94.66</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>95.174999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>95.015000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>95.405000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>95.56</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>95.685000000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>96.345000000000013</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>96.414999999999992</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>96.305000000000021</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>96.21</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95.890000000000015</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95.65</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.530000000000015</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>95.79</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95.434999999999988</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95.585000000000008</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>95.06</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>95.33</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>95.084999999999994</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>94.759999999999962</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.820000000000007</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94.70999999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>94.45</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="128059264"/>
+        <c:axId val="128060800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="128059264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128060800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="128060800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128059264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -833,7 +2211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V961"/>
   <sheetViews>
-    <sheetView topLeftCell="A917" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S1" sqref="S1:V961"/>
     </sheetView>
   </sheetViews>
@@ -67157,8 +68535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -68243,5 +69621,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>